<commit_message>
Fin des problèmes de base
</commit_message>
<xml_diff>
--- a/bdd_excel/Avis.xlsx
+++ b/bdd_excel/Avis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/florianbour/Desktop/ENSEIRB/2A/SGBD/sgbd-jeux/bdd_excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A78E9F9-C5DE-DF42-90E8-E08E3D857A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0192813-C828-C44F-A980-4D8EEF9EBA82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16000" xr2:uid="{FFAC0233-3D28-634B-9D7E-2085D8CE6967}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="495">
   <si>
     <t>id_avis</t>
   </si>
@@ -933,12 +933,6 @@
   </si>
   <si>
     <t>'24-NOV-2021'</t>
-  </si>
-  <si>
-    <t>"Minimal"</t>
-  </si>
-  <si>
-    <t>'03-APR-2020'</t>
   </si>
   <si>
     <t>"Développé"</t>
@@ -1875,10 +1869,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7554BF90-C002-4843-AC84-EB706920A8E3}">
-  <dimension ref="A1:G251"/>
+  <dimension ref="A1:G250"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A206" workbookViewId="0">
+      <selection activeCell="F215" sqref="F215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5338,7 +5332,7 @@
         <v>150</v>
       </c>
       <c r="B151">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C151" t="s">
         <v>300</v>
@@ -5347,10 +5341,10 @@
         <v>301</v>
       </c>
       <c r="E151">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F151">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G151">
         <v>58</v>
@@ -5370,10 +5364,10 @@
         <v>303</v>
       </c>
       <c r="E152">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="F152">
-        <v>21</v>
+        <v>102</v>
       </c>
       <c r="G152">
         <v>58</v>
@@ -5384,7 +5378,7 @@
         <v>152</v>
       </c>
       <c r="B153">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C153" t="s">
         <v>304</v>
@@ -5393,10 +5387,10 @@
         <v>305</v>
       </c>
       <c r="E153">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="F153">
-        <v>102</v>
+        <v>35</v>
       </c>
       <c r="G153">
         <v>58</v>
@@ -5407,7 +5401,7 @@
         <v>153</v>
       </c>
       <c r="B154">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C154" t="s">
         <v>306</v>
@@ -5416,10 +5410,10 @@
         <v>307</v>
       </c>
       <c r="E154">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="F154">
-        <v>35</v>
+        <v>99</v>
       </c>
       <c r="G154">
         <v>58</v>
@@ -5430,7 +5424,7 @@
         <v>154</v>
       </c>
       <c r="B155">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C155" t="s">
         <v>308</v>
@@ -5439,10 +5433,10 @@
         <v>309</v>
       </c>
       <c r="E155">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F155">
-        <v>99</v>
+        <v>66</v>
       </c>
       <c r="G155">
         <v>58</v>
@@ -5453,7 +5447,7 @@
         <v>155</v>
       </c>
       <c r="B156">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C156" t="s">
         <v>310</v>
@@ -5462,10 +5456,10 @@
         <v>311</v>
       </c>
       <c r="E156">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="F156">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="G156">
         <v>58</v>
@@ -5476,7 +5470,7 @@
         <v>156</v>
       </c>
       <c r="B157">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C157" t="s">
         <v>312</v>
@@ -5485,10 +5479,10 @@
         <v>313</v>
       </c>
       <c r="E157">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="F157">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="G157">
         <v>58</v>
@@ -5499,7 +5493,7 @@
         <v>157</v>
       </c>
       <c r="B158">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C158" t="s">
         <v>314</v>
@@ -5508,10 +5502,10 @@
         <v>315</v>
       </c>
       <c r="E158">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="F158">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="G158">
         <v>58</v>
@@ -5522,7 +5516,7 @@
         <v>158</v>
       </c>
       <c r="B159">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C159" t="s">
         <v>316</v>
@@ -5531,10 +5525,10 @@
         <v>317</v>
       </c>
       <c r="E159">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="F159">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="G159">
         <v>58</v>
@@ -5545,7 +5539,7 @@
         <v>159</v>
       </c>
       <c r="B160">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C160" t="s">
         <v>318</v>
@@ -5554,13 +5548,13 @@
         <v>319</v>
       </c>
       <c r="E160">
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="F160">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="G160">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.2">
@@ -5568,7 +5562,7 @@
         <v>160</v>
       </c>
       <c r="B161">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C161" t="s">
         <v>320</v>
@@ -5577,10 +5571,10 @@
         <v>321</v>
       </c>
       <c r="E161">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="F161">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G161">
         <v>59</v>
@@ -5591,7 +5585,7 @@
         <v>161</v>
       </c>
       <c r="B162">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C162" t="s">
         <v>322</v>
@@ -5600,10 +5594,10 @@
         <v>323</v>
       </c>
       <c r="E162">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="F162">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G162">
         <v>59</v>
@@ -5614,7 +5608,7 @@
         <v>162</v>
       </c>
       <c r="B163">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C163" t="s">
         <v>324</v>
@@ -5623,10 +5617,10 @@
         <v>325</v>
       </c>
       <c r="E163">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="F163">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="G163">
         <v>59</v>
@@ -5637,19 +5631,19 @@
         <v>163</v>
       </c>
       <c r="B164">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C164" t="s">
         <v>326</v>
       </c>
       <c r="D164" t="s">
-        <v>327</v>
+        <v>118</v>
       </c>
       <c r="E164">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F164">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="G164">
         <v>59</v>
@@ -5660,19 +5654,19 @@
         <v>164</v>
       </c>
       <c r="B165">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C165" t="s">
+        <v>327</v>
+      </c>
+      <c r="D165" t="s">
         <v>328</v>
       </c>
-      <c r="D165" t="s">
-        <v>118</v>
-      </c>
       <c r="E165">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F165">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="G165">
         <v>59</v>
@@ -5683,7 +5677,7 @@
         <v>165</v>
       </c>
       <c r="B166">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C166" t="s">
         <v>329</v>
@@ -5692,10 +5686,10 @@
         <v>330</v>
       </c>
       <c r="E166">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="F166">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="G166">
         <v>59</v>
@@ -5706,7 +5700,7 @@
         <v>166</v>
       </c>
       <c r="B167">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C167" t="s">
         <v>331</v>
@@ -5715,10 +5709,10 @@
         <v>332</v>
       </c>
       <c r="E167">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="F167">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="G167">
         <v>59</v>
@@ -5729,19 +5723,19 @@
         <v>167</v>
       </c>
       <c r="B168">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C168" t="s">
         <v>333</v>
       </c>
       <c r="D168" t="s">
-        <v>334</v>
+        <v>72</v>
       </c>
       <c r="E168">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="F168">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="G168">
         <v>59</v>
@@ -5752,16 +5746,16 @@
         <v>168</v>
       </c>
       <c r="B169">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C169" t="s">
+        <v>334</v>
+      </c>
+      <c r="D169" t="s">
         <v>335</v>
       </c>
-      <c r="D169" t="s">
-        <v>72</v>
-      </c>
       <c r="E169">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F169">
         <v>26</v>
@@ -5775,7 +5769,7 @@
         <v>169</v>
       </c>
       <c r="B170">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C170" t="s">
         <v>336</v>
@@ -5784,10 +5778,10 @@
         <v>337</v>
       </c>
       <c r="E170">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F170">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="G170">
         <v>59</v>
@@ -5798,7 +5792,7 @@
         <v>170</v>
       </c>
       <c r="B171">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C171" t="s">
         <v>338</v>
@@ -5807,10 +5801,10 @@
         <v>339</v>
       </c>
       <c r="E171">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="F171">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="G171">
         <v>59</v>
@@ -5821,7 +5815,7 @@
         <v>171</v>
       </c>
       <c r="B172">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C172" t="s">
         <v>340</v>
@@ -5830,10 +5824,10 @@
         <v>341</v>
       </c>
       <c r="E172">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="F172">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="G172">
         <v>59</v>
@@ -5844,7 +5838,7 @@
         <v>172</v>
       </c>
       <c r="B173">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C173" t="s">
         <v>342</v>
@@ -5853,10 +5847,10 @@
         <v>343</v>
       </c>
       <c r="E173">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="F173">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="G173">
         <v>59</v>
@@ -5867,7 +5861,7 @@
         <v>173</v>
       </c>
       <c r="B174">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C174" t="s">
         <v>344</v>
@@ -5876,10 +5870,10 @@
         <v>345</v>
       </c>
       <c r="E174">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="F174">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="G174">
         <v>59</v>
@@ -5890,7 +5884,7 @@
         <v>174</v>
       </c>
       <c r="B175">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C175" t="s">
         <v>346</v>
@@ -5899,10 +5893,10 @@
         <v>347</v>
       </c>
       <c r="E175">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="F175">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="G175">
         <v>59</v>
@@ -5913,7 +5907,7 @@
         <v>175</v>
       </c>
       <c r="B176">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C176" t="s">
         <v>348</v>
@@ -5922,10 +5916,10 @@
         <v>349</v>
       </c>
       <c r="E176">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F176">
-        <v>84</v>
+        <v>37</v>
       </c>
       <c r="G176">
         <v>59</v>
@@ -5936,19 +5930,19 @@
         <v>176</v>
       </c>
       <c r="B177">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C177" t="s">
         <v>350</v>
       </c>
       <c r="D177" t="s">
-        <v>351</v>
+        <v>50</v>
       </c>
       <c r="E177">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="F177">
-        <v>37</v>
+        <v>90</v>
       </c>
       <c r="G177">
         <v>59</v>
@@ -5959,19 +5953,19 @@
         <v>177</v>
       </c>
       <c r="B178">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C178" t="s">
+        <v>351</v>
+      </c>
+      <c r="D178" t="s">
         <v>352</v>
       </c>
-      <c r="D178" t="s">
-        <v>50</v>
-      </c>
       <c r="E178">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F178">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="G178">
         <v>59</v>
@@ -5982,7 +5976,7 @@
         <v>178</v>
       </c>
       <c r="B179">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C179" t="s">
         <v>353</v>
@@ -5991,10 +5985,10 @@
         <v>354</v>
       </c>
       <c r="E179">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="F179">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="G179">
         <v>59</v>
@@ -6005,7 +5999,7 @@
         <v>179</v>
       </c>
       <c r="B180">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C180" t="s">
         <v>355</v>
@@ -6014,13 +6008,13 @@
         <v>356</v>
       </c>
       <c r="E180">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="F180">
-        <v>92</v>
+        <v>1</v>
       </c>
       <c r="G180">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.2">
@@ -6028,7 +6022,7 @@
         <v>180</v>
       </c>
       <c r="B181">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C181" t="s">
         <v>357</v>
@@ -6037,10 +6031,10 @@
         <v>358</v>
       </c>
       <c r="E181">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="F181">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="G181">
         <v>60</v>
@@ -6051,7 +6045,7 @@
         <v>181</v>
       </c>
       <c r="B182">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C182" t="s">
         <v>359</v>
@@ -6060,10 +6054,10 @@
         <v>360</v>
       </c>
       <c r="E182">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="F182">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="G182">
         <v>60</v>
@@ -6074,7 +6068,7 @@
         <v>182</v>
       </c>
       <c r="B183">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C183" t="s">
         <v>361</v>
@@ -6083,13 +6077,13 @@
         <v>362</v>
       </c>
       <c r="E183">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F183">
-        <v>91</v>
+        <v>18</v>
       </c>
       <c r="G183">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.2">
@@ -6097,7 +6091,7 @@
         <v>183</v>
       </c>
       <c r="B184">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C184" t="s">
         <v>363</v>
@@ -6106,10 +6100,10 @@
         <v>364</v>
       </c>
       <c r="E184">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F184">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="G184">
         <v>61</v>
@@ -6120,7 +6114,7 @@
         <v>184</v>
       </c>
       <c r="B185">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C185" t="s">
         <v>365</v>
@@ -6129,10 +6123,10 @@
         <v>366</v>
       </c>
       <c r="E185">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="F185">
-        <v>54</v>
+        <v>11</v>
       </c>
       <c r="G185">
         <v>61</v>
@@ -6152,13 +6146,13 @@
         <v>368</v>
       </c>
       <c r="E186">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="F186">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="G186">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.2">
@@ -6166,7 +6160,7 @@
         <v>186</v>
       </c>
       <c r="B187">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C187" t="s">
         <v>369</v>
@@ -6175,10 +6169,10 @@
         <v>370</v>
       </c>
       <c r="E187">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="F187">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="G187">
         <v>62</v>
@@ -6189,7 +6183,7 @@
         <v>187</v>
       </c>
       <c r="B188">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C188" t="s">
         <v>371</v>
@@ -6198,13 +6192,13 @@
         <v>372</v>
       </c>
       <c r="E188">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F188">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="G188">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.2">
@@ -6212,7 +6206,7 @@
         <v>188</v>
       </c>
       <c r="B189">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C189" t="s">
         <v>373</v>
@@ -6221,10 +6215,10 @@
         <v>374</v>
       </c>
       <c r="E189">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F189">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="G189">
         <v>64</v>
@@ -6235,7 +6229,7 @@
         <v>189</v>
       </c>
       <c r="B190">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C190" t="s">
         <v>375</v>
@@ -6244,10 +6238,10 @@
         <v>376</v>
       </c>
       <c r="E190">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="F190">
-        <v>89</v>
+        <v>41</v>
       </c>
       <c r="G190">
         <v>64</v>
@@ -6258,7 +6252,7 @@
         <v>190</v>
       </c>
       <c r="B191">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C191" t="s">
         <v>377</v>
@@ -6267,10 +6261,10 @@
         <v>378</v>
       </c>
       <c r="E191">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="F191">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="G191">
         <v>64</v>
@@ -6281,7 +6275,7 @@
         <v>191</v>
       </c>
       <c r="B192">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C192" t="s">
         <v>379</v>
@@ -6290,13 +6284,13 @@
         <v>380</v>
       </c>
       <c r="E192">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="F192">
-        <v>82</v>
+        <v>13</v>
       </c>
       <c r="G192">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.2">
@@ -6304,7 +6298,7 @@
         <v>192</v>
       </c>
       <c r="B193">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C193" t="s">
         <v>381</v>
@@ -6313,10 +6307,10 @@
         <v>382</v>
       </c>
       <c r="E193">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="F193">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="G193">
         <v>65</v>
@@ -6327,7 +6321,7 @@
         <v>193</v>
       </c>
       <c r="B194">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C194" t="s">
         <v>383</v>
@@ -6336,13 +6330,13 @@
         <v>384</v>
       </c>
       <c r="E194">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="F194">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="G194">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.2">
@@ -6350,7 +6344,7 @@
         <v>194</v>
       </c>
       <c r="B195">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C195" t="s">
         <v>385</v>
@@ -6359,10 +6353,10 @@
         <v>386</v>
       </c>
       <c r="E195">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="F195">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="G195">
         <v>66</v>
@@ -6373,7 +6367,7 @@
         <v>195</v>
       </c>
       <c r="B196">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C196" t="s">
         <v>387</v>
@@ -6382,10 +6376,10 @@
         <v>388</v>
       </c>
       <c r="E196">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F196">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="G196">
         <v>66</v>
@@ -6396,7 +6390,7 @@
         <v>196</v>
       </c>
       <c r="B197">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C197" t="s">
         <v>389</v>
@@ -6405,7 +6399,7 @@
         <v>390</v>
       </c>
       <c r="E197">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F197">
         <v>99</v>
@@ -6419,7 +6413,7 @@
         <v>197</v>
       </c>
       <c r="B198">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="C198" t="s">
         <v>391</v>
@@ -6428,10 +6422,10 @@
         <v>392</v>
       </c>
       <c r="E198">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="F198">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="G198">
         <v>66</v>
@@ -6442,7 +6436,7 @@
         <v>198</v>
       </c>
       <c r="B199">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C199" t="s">
         <v>393</v>
@@ -6451,10 +6445,10 @@
         <v>394</v>
       </c>
       <c r="E199">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="F199">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="G199">
         <v>66</v>
@@ -6465,7 +6459,7 @@
         <v>199</v>
       </c>
       <c r="B200">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C200" t="s">
         <v>395</v>
@@ -6474,10 +6468,10 @@
         <v>396</v>
       </c>
       <c r="E200">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="F200">
-        <v>31</v>
+        <v>100</v>
       </c>
       <c r="G200">
         <v>66</v>
@@ -6488,19 +6482,19 @@
         <v>200</v>
       </c>
       <c r="B201">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C201" t="s">
         <v>397</v>
       </c>
       <c r="D201" t="s">
-        <v>398</v>
+        <v>215</v>
       </c>
       <c r="E201">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="F201">
-        <v>100</v>
+        <v>61</v>
       </c>
       <c r="G201">
         <v>66</v>
@@ -6511,19 +6505,19 @@
         <v>201</v>
       </c>
       <c r="B202">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C202" t="s">
+        <v>398</v>
+      </c>
+      <c r="D202" t="s">
         <v>399</v>
       </c>
-      <c r="D202" t="s">
-        <v>215</v>
-      </c>
       <c r="E202">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="F202">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="G202">
         <v>66</v>
@@ -6534,7 +6528,7 @@
         <v>202</v>
       </c>
       <c r="B203">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C203" t="s">
         <v>400</v>
@@ -6543,10 +6537,10 @@
         <v>401</v>
       </c>
       <c r="E203">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="F203">
-        <v>82</v>
+        <v>15</v>
       </c>
       <c r="G203">
         <v>66</v>
@@ -6566,10 +6560,10 @@
         <v>403</v>
       </c>
       <c r="E204">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="F204">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G204">
         <v>66</v>
@@ -6580,7 +6574,7 @@
         <v>204</v>
       </c>
       <c r="B205">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C205" t="s">
         <v>404</v>
@@ -6589,10 +6583,10 @@
         <v>405</v>
       </c>
       <c r="E205">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F205">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G205">
         <v>66</v>
@@ -6603,7 +6597,7 @@
         <v>205</v>
       </c>
       <c r="B206">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C206" t="s">
         <v>406</v>
@@ -6612,10 +6606,10 @@
         <v>407</v>
       </c>
       <c r="E206">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F206">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="G206">
         <v>66</v>
@@ -6635,10 +6629,10 @@
         <v>409</v>
       </c>
       <c r="E207">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="F207">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="G207">
         <v>66</v>
@@ -6649,7 +6643,7 @@
         <v>207</v>
       </c>
       <c r="B208">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C208" t="s">
         <v>410</v>
@@ -6658,10 +6652,10 @@
         <v>411</v>
       </c>
       <c r="E208">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="F208">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="G208">
         <v>66</v>
@@ -6672,7 +6666,7 @@
         <v>208</v>
       </c>
       <c r="B209">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C209" t="s">
         <v>412</v>
@@ -6681,10 +6675,10 @@
         <v>413</v>
       </c>
       <c r="E209">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F209">
-        <v>84</v>
+        <v>50</v>
       </c>
       <c r="G209">
         <v>66</v>
@@ -6695,7 +6689,7 @@
         <v>209</v>
       </c>
       <c r="B210">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C210" t="s">
         <v>414</v>
@@ -6704,13 +6698,13 @@
         <v>415</v>
       </c>
       <c r="E210">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F210">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G210">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.2">
@@ -6718,7 +6712,7 @@
         <v>210</v>
       </c>
       <c r="B211">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C211" t="s">
         <v>416</v>
@@ -6727,13 +6721,13 @@
         <v>417</v>
       </c>
       <c r="E211">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F211">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="G211">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.2">
@@ -6741,7 +6735,7 @@
         <v>211</v>
       </c>
       <c r="B212">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C212" t="s">
         <v>418</v>
@@ -6750,10 +6744,10 @@
         <v>419</v>
       </c>
       <c r="E212">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F212">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G212">
         <v>69</v>
@@ -6764,7 +6758,7 @@
         <v>212</v>
       </c>
       <c r="B213">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C213" t="s">
         <v>420</v>
@@ -6773,13 +6767,13 @@
         <v>421</v>
       </c>
       <c r="E213">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="F213">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="G213">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.2">
@@ -6787,7 +6781,7 @@
         <v>213</v>
       </c>
       <c r="B214">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C214" t="s">
         <v>422</v>
@@ -6796,10 +6790,10 @@
         <v>423</v>
       </c>
       <c r="E214">
+        <v>29</v>
+      </c>
+      <c r="F214">
         <v>1</v>
-      </c>
-      <c r="F214">
-        <v>55</v>
       </c>
       <c r="G214">
         <v>70</v>
@@ -6810,7 +6804,7 @@
         <v>214</v>
       </c>
       <c r="B215">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C215" t="s">
         <v>424</v>
@@ -6819,10 +6813,10 @@
         <v>425</v>
       </c>
       <c r="E215">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="F215">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="G215">
         <v>70</v>
@@ -6833,7 +6827,7 @@
         <v>215</v>
       </c>
       <c r="B216">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C216" t="s">
         <v>426</v>
@@ -6842,10 +6836,10 @@
         <v>427</v>
       </c>
       <c r="E216">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="F216">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G216">
         <v>70</v>
@@ -6856,7 +6850,7 @@
         <v>216</v>
       </c>
       <c r="B217">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C217" t="s">
         <v>428</v>
@@ -6865,10 +6859,10 @@
         <v>429</v>
       </c>
       <c r="E217">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="F217">
-        <v>34</v>
+        <v>73</v>
       </c>
       <c r="G217">
         <v>70</v>
@@ -6879,7 +6873,7 @@
         <v>217</v>
       </c>
       <c r="B218">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C218" t="s">
         <v>430</v>
@@ -6888,10 +6882,10 @@
         <v>431</v>
       </c>
       <c r="E218">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="F218">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="G218">
         <v>70</v>
@@ -6902,7 +6896,7 @@
         <v>218</v>
       </c>
       <c r="B219">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C219" t="s">
         <v>432</v>
@@ -6911,10 +6905,10 @@
         <v>433</v>
       </c>
       <c r="E219">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="F219">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="G219">
         <v>70</v>
@@ -6925,7 +6919,7 @@
         <v>219</v>
       </c>
       <c r="B220">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C220" t="s">
         <v>434</v>
@@ -6934,10 +6928,10 @@
         <v>435</v>
       </c>
       <c r="E220">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F220">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="G220">
         <v>70</v>
@@ -6948,7 +6942,7 @@
         <v>220</v>
       </c>
       <c r="B221">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C221" t="s">
         <v>436</v>
@@ -6957,10 +6951,10 @@
         <v>437</v>
       </c>
       <c r="E221">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F221">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G221">
         <v>70</v>
@@ -6971,7 +6965,7 @@
         <v>221</v>
       </c>
       <c r="B222">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C222" t="s">
         <v>438</v>
@@ -6980,13 +6974,13 @@
         <v>439</v>
       </c>
       <c r="E222">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F222">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="G222">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.2">
@@ -6994,7 +6988,7 @@
         <v>222</v>
       </c>
       <c r="B223">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C223" t="s">
         <v>440</v>
@@ -7003,10 +6997,10 @@
         <v>441</v>
       </c>
       <c r="E223">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="F223">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="G223">
         <v>72</v>
@@ -7017,19 +7011,19 @@
         <v>223</v>
       </c>
       <c r="B224">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C224" t="s">
         <v>442</v>
       </c>
       <c r="D224" t="s">
-        <v>443</v>
+        <v>291</v>
       </c>
       <c r="E224">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F224">
-        <v>86</v>
+        <v>36</v>
       </c>
       <c r="G224">
         <v>72</v>
@@ -7040,22 +7034,22 @@
         <v>224</v>
       </c>
       <c r="B225">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C225" t="s">
+        <v>443</v>
+      </c>
+      <c r="D225" t="s">
         <v>444</v>
       </c>
-      <c r="D225" t="s">
-        <v>291</v>
-      </c>
       <c r="E225">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="F225">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="G225">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.2">
@@ -7063,7 +7057,7 @@
         <v>225</v>
       </c>
       <c r="B226">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C226" t="s">
         <v>445</v>
@@ -7072,13 +7066,13 @@
         <v>446</v>
       </c>
       <c r="E226">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="F226">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="G226">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.2">
@@ -7086,7 +7080,7 @@
         <v>226</v>
       </c>
       <c r="B227">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C227" t="s">
         <v>447</v>
@@ -7095,10 +7089,10 @@
         <v>448</v>
       </c>
       <c r="E227">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F227">
-        <v>78</v>
+        <v>20</v>
       </c>
       <c r="G227">
         <v>74</v>
@@ -7109,7 +7103,7 @@
         <v>227</v>
       </c>
       <c r="B228">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C228" t="s">
         <v>449</v>
@@ -7118,10 +7112,10 @@
         <v>450</v>
       </c>
       <c r="E228">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="F228">
-        <v>20</v>
+        <v>99</v>
       </c>
       <c r="G228">
         <v>74</v>
@@ -7132,7 +7126,7 @@
         <v>228</v>
       </c>
       <c r="B229">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C229" t="s">
         <v>451</v>
@@ -7141,13 +7135,13 @@
         <v>452</v>
       </c>
       <c r="E229">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F229">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="G229">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.2">
@@ -7155,7 +7149,7 @@
         <v>229</v>
       </c>
       <c r="B230">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C230" t="s">
         <v>453</v>
@@ -7164,13 +7158,13 @@
         <v>454</v>
       </c>
       <c r="E230">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="F230">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="G230">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.2">
@@ -7178,7 +7172,7 @@
         <v>230</v>
       </c>
       <c r="B231">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C231" t="s">
         <v>455</v>
@@ -7187,13 +7181,13 @@
         <v>456</v>
       </c>
       <c r="E231">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F231">
-        <v>97</v>
+        <v>48</v>
       </c>
       <c r="G231">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.2">
@@ -7201,7 +7195,7 @@
         <v>231</v>
       </c>
       <c r="B232">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C232" t="s">
         <v>457</v>
@@ -7210,10 +7204,10 @@
         <v>458</v>
       </c>
       <c r="E232">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F232">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="G232">
         <v>77</v>
@@ -7224,7 +7218,7 @@
         <v>232</v>
       </c>
       <c r="B233">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C233" t="s">
         <v>459</v>
@@ -7233,13 +7227,13 @@
         <v>460</v>
       </c>
       <c r="E233">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="F233">
-        <v>71</v>
+        <v>12</v>
       </c>
       <c r="G233">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.2">
@@ -7247,7 +7241,7 @@
         <v>233</v>
       </c>
       <c r="B234">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C234" t="s">
         <v>461</v>
@@ -7256,13 +7250,13 @@
         <v>462</v>
       </c>
       <c r="E234">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F234">
-        <v>12</v>
+        <v>97</v>
       </c>
       <c r="G234">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.2">
@@ -7270,7 +7264,7 @@
         <v>234</v>
       </c>
       <c r="B235">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C235" t="s">
         <v>463</v>
@@ -7279,13 +7273,13 @@
         <v>464</v>
       </c>
       <c r="E235">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F235">
-        <v>97</v>
+        <v>68</v>
       </c>
       <c r="G235">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.2">
@@ -7293,7 +7287,7 @@
         <v>235</v>
       </c>
       <c r="B236">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C236" t="s">
         <v>465</v>
@@ -7302,10 +7296,10 @@
         <v>466</v>
       </c>
       <c r="E236">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="F236">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="G236">
         <v>84</v>
@@ -7316,7 +7310,7 @@
         <v>236</v>
       </c>
       <c r="B237">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C237" t="s">
         <v>467</v>
@@ -7325,10 +7319,10 @@
         <v>468</v>
       </c>
       <c r="E237">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="F237">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="G237">
         <v>84</v>
@@ -7339,7 +7333,7 @@
         <v>237</v>
       </c>
       <c r="B238">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C238" t="s">
         <v>469</v>
@@ -7348,10 +7342,10 @@
         <v>470</v>
       </c>
       <c r="E238">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="F238">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G238">
         <v>84</v>
@@ -7362,7 +7356,7 @@
         <v>238</v>
       </c>
       <c r="B239">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C239" t="s">
         <v>471</v>
@@ -7371,10 +7365,10 @@
         <v>472</v>
       </c>
       <c r="E239">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="F239">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="G239">
         <v>84</v>
@@ -7385,7 +7379,7 @@
         <v>239</v>
       </c>
       <c r="B240">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C240" t="s">
         <v>473</v>
@@ -7394,13 +7388,13 @@
         <v>474</v>
       </c>
       <c r="E240">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="F240">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="G240">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.2">
@@ -7417,10 +7411,10 @@
         <v>476</v>
       </c>
       <c r="E241">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="F241">
-        <v>69</v>
+        <v>9</v>
       </c>
       <c r="G241">
         <v>87</v>
@@ -7431,7 +7425,7 @@
         <v>241</v>
       </c>
       <c r="B242">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C242" t="s">
         <v>477</v>
@@ -7440,10 +7434,10 @@
         <v>478</v>
       </c>
       <c r="E242">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="F242">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G242">
         <v>87</v>
@@ -7454,7 +7448,7 @@
         <v>242</v>
       </c>
       <c r="B243">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C243" t="s">
         <v>479</v>
@@ -7463,13 +7457,13 @@
         <v>480</v>
       </c>
       <c r="E243">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="F243">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G243">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.2">
@@ -7477,7 +7471,7 @@
         <v>243</v>
       </c>
       <c r="B244">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C244" t="s">
         <v>481</v>
@@ -7486,10 +7480,10 @@
         <v>482</v>
       </c>
       <c r="E244">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F244">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="G244">
         <v>88</v>
@@ -7500,7 +7494,7 @@
         <v>244</v>
       </c>
       <c r="B245">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C245" t="s">
         <v>483</v>
@@ -7509,10 +7503,10 @@
         <v>484</v>
       </c>
       <c r="E245">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="F245">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="G245">
         <v>88</v>
@@ -7523,7 +7517,7 @@
         <v>245</v>
       </c>
       <c r="B246">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C246" t="s">
         <v>485</v>
@@ -7532,10 +7526,10 @@
         <v>486</v>
       </c>
       <c r="E246">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F246">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="G246">
         <v>88</v>
@@ -7546,7 +7540,7 @@
         <v>246</v>
       </c>
       <c r="B247">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C247" t="s">
         <v>487</v>
@@ -7555,13 +7549,13 @@
         <v>488</v>
       </c>
       <c r="E247">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="F247">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="G247">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.2">
@@ -7569,7 +7563,7 @@
         <v>247</v>
       </c>
       <c r="B248">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C248" t="s">
         <v>489</v>
@@ -7578,10 +7572,10 @@
         <v>490</v>
       </c>
       <c r="E248">
+        <v>20</v>
+      </c>
+      <c r="F248">
         <v>21</v>
-      </c>
-      <c r="F248">
-        <v>37</v>
       </c>
       <c r="G248">
         <v>91</v>
@@ -7592,7 +7586,7 @@
         <v>248</v>
       </c>
       <c r="B249">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C249" t="s">
         <v>491</v>
@@ -7601,10 +7595,10 @@
         <v>492</v>
       </c>
       <c r="E249">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="F249">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G249">
         <v>91</v>
@@ -7615,7 +7609,7 @@
         <v>249</v>
       </c>
       <c r="B250">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C250" t="s">
         <v>493</v>
@@ -7624,35 +7618,12 @@
         <v>494</v>
       </c>
       <c r="E250">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="F250">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="G250">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A251">
-        <v>250</v>
-      </c>
-      <c r="B251">
-        <v>3</v>
-      </c>
-      <c r="C251" t="s">
-        <v>495</v>
-      </c>
-      <c r="D251" t="s">
-        <v>496</v>
-      </c>
-      <c r="E251">
-        <v>4</v>
-      </c>
-      <c r="F251">
-        <v>77</v>
-      </c>
-      <c r="G251">
         <v>92</v>
       </c>
     </row>

</xml_diff>